<commit_message>
[RF GEN] Femto release version
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V1.0/RF-GEN-CPU_PinMap_20190429.xlsx
+++ b/1_Schematic/Build V1.0/RF-GEN-CPU_PinMap_20190429.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52317E15-C001-49D1-96F6-F0C2F9F15F7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329CA47E-A5D1-4E5B-87C1-F570004C4048}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="626">
   <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2391,14 +2391,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PB6_BIAS_ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PB7_GPIO_ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HIGH Active</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2446,6 +2438,66 @@
   <si>
     <t>Buck output Voltage monitor</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과전류 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PW_IS_AD : 2.01V 이상(ADC : 2496)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN 동작 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN_PW_AD : 0.51V 이하(ADC : 634)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forward Power monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflected Power monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Transistor Over(65℃) temp 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Temperature</t>
+  </si>
+  <si>
+    <t>25KHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN 동작 제어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Cable detect error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case detect error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50KHz</t>
+  </si>
+  <si>
+    <t>LCD와 통신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF PCB의 Bias control</t>
+  </si>
+  <si>
+    <t>RF 48V 전원 control</t>
   </si>
 </sst>
 </file>
@@ -3067,7 +3119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="355">
+  <cellXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3958,6 +4010,108 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3976,9 +4130,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3987,57 +4138,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4057,53 +4157,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4705,8 +4766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AB95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4763,10 +4824,10 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B3" s="316" t="s">
+      <c r="B3" s="334" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="317"/>
+      <c r="C3" s="335"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -4799,10 +4860,10 @@
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B4" s="318" t="s">
+      <c r="B4" s="336" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="319"/>
+      <c r="C4" s="337"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -4837,10 +4898,10 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B5" s="318" t="s">
+      <c r="B5" s="336" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="319"/>
+      <c r="C5" s="337"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -4877,10 +4938,10 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B6" s="318" t="s">
+      <c r="B6" s="336" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="319"/>
+      <c r="C6" s="337"/>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
@@ -4909,10 +4970,10 @@
       <c r="U6" s="10"/>
     </row>
     <row r="7" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="320" t="s">
+      <c r="B7" s="338" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="321"/>
+      <c r="C7" s="339"/>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
@@ -5081,23 +5142,23 @@
     </row>
     <row r="13" spans="2:24" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="14" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="311" t="s">
+      <c r="B14" s="345" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="312"/>
-      <c r="D14" s="312" t="s">
+      <c r="C14" s="332"/>
+      <c r="D14" s="332" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="312" t="s">
+      <c r="E14" s="332" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="332"/>
-      <c r="G14" s="306" t="s">
+      <c r="F14" s="333"/>
+      <c r="G14" s="340" t="s">
         <v>562</v>
       </c>
-      <c r="H14" s="307"/>
-      <c r="I14" s="307"/>
-      <c r="J14" s="308"/>
+      <c r="H14" s="341"/>
+      <c r="I14" s="341"/>
+      <c r="J14" s="342"/>
       <c r="K14" s="302"/>
       <c r="L14" s="322" t="s">
         <v>399</v>
@@ -5128,7 +5189,7 @@
       <c r="C15" s="114" t="s">
         <v>377</v>
       </c>
-      <c r="D15" s="313"/>
+      <c r="D15" s="346"/>
       <c r="E15" s="114" t="s">
         <v>162</v>
       </c>
@@ -5147,7 +5208,7 @@
       <c r="J15" s="255" t="s">
         <v>0</v>
       </c>
-      <c r="K15" s="339"/>
+      <c r="K15" s="306"/>
       <c r="L15" s="138" t="s">
         <v>401</v>
       </c>
@@ -5198,17 +5259,17 @@
       <c r="D16" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="309" t="s">
+      <c r="E16" s="343" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="310"/>
+      <c r="F16" s="344"/>
       <c r="G16" s="33"/>
       <c r="H16" s="253"/>
       <c r="I16" s="289" t="s">
         <v>563</v>
       </c>
       <c r="J16" s="254"/>
-      <c r="K16" s="340"/>
+      <c r="K16" s="307"/>
       <c r="L16" s="273"/>
       <c r="M16" s="143"/>
       <c r="N16" s="144"/>
@@ -5243,7 +5304,7 @@
       <c r="H17" s="287"/>
       <c r="I17" s="287"/>
       <c r="J17" s="294"/>
-      <c r="K17" s="341"/>
+      <c r="K17" s="308"/>
       <c r="L17" s="274" t="s">
         <v>407</v>
       </c>
@@ -5300,7 +5361,7 @@
         <v>564</v>
       </c>
       <c r="J18" s="97"/>
-      <c r="K18" s="342"/>
+      <c r="K18" s="309"/>
       <c r="L18" s="274" t="s">
         <v>409</v>
       </c>
@@ -5357,7 +5418,7 @@
         <v>564</v>
       </c>
       <c r="J19" s="97"/>
-      <c r="K19" s="342"/>
+      <c r="K19" s="309"/>
       <c r="L19" s="274" t="s">
         <v>409</v>
       </c>
@@ -5414,7 +5475,7 @@
         <v>565</v>
       </c>
       <c r="J20" s="97"/>
-      <c r="K20" s="342"/>
+      <c r="K20" s="309"/>
       <c r="L20" s="274" t="s">
         <v>409</v>
       </c>
@@ -5471,7 +5532,7 @@
         <v>565</v>
       </c>
       <c r="J21" s="97"/>
-      <c r="K21" s="342"/>
+      <c r="K21" s="309"/>
       <c r="L21" s="274" t="s">
         <v>409</v>
       </c>
@@ -5516,17 +5577,17 @@
       <c r="D22" s="104" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="314" t="s">
+      <c r="E22" s="347" t="s">
         <v>98</v>
       </c>
-      <c r="F22" s="315"/>
+      <c r="F22" s="348"/>
       <c r="G22" s="47"/>
       <c r="H22" s="256"/>
       <c r="I22" s="256" t="s">
         <v>566</v>
       </c>
       <c r="J22" s="257"/>
-      <c r="K22" s="343"/>
+      <c r="K22" s="310"/>
       <c r="L22" s="275" t="s">
         <v>411</v>
       </c>
@@ -5587,10 +5648,10 @@
         <v>568</v>
       </c>
       <c r="J23" s="41" t="s">
+        <v>605</v>
+      </c>
+      <c r="K23" s="321" t="s">
         <v>607</v>
-      </c>
-      <c r="K23" s="354" t="s">
-        <v>609</v>
       </c>
       <c r="L23" s="276" t="s">
         <v>414</v>
@@ -5651,13 +5712,13 @@
         <v>18</v>
       </c>
       <c r="I24" s="39" t="s">
+        <v>606</v>
+      </c>
+      <c r="J24" s="298" t="s">
+        <v>609</v>
+      </c>
+      <c r="K24" s="321" t="s">
         <v>608</v>
-      </c>
-      <c r="J24" s="298" t="s">
-        <v>611</v>
-      </c>
-      <c r="K24" s="354" t="s">
-        <v>610</v>
       </c>
       <c r="L24" s="277" t="s">
         <v>420</v>
@@ -5718,8 +5779,12 @@
       <c r="I25" s="39" t="s">
         <v>537</v>
       </c>
-      <c r="J25" s="298"/>
-      <c r="K25" s="344"/>
+      <c r="J25" s="298" t="s">
+        <v>610</v>
+      </c>
+      <c r="K25" s="355" t="s">
+        <v>611</v>
+      </c>
       <c r="L25" s="277" t="s">
         <v>420</v>
       </c>
@@ -5779,8 +5844,12 @@
       <c r="I26" s="39" t="s">
         <v>569</v>
       </c>
-      <c r="J26" s="298"/>
-      <c r="K26" s="344"/>
+      <c r="J26" s="298" t="s">
+        <v>612</v>
+      </c>
+      <c r="K26" s="355" t="s">
+        <v>613</v>
+      </c>
       <c r="L26" s="277" t="s">
         <v>420</v>
       </c>
@@ -5833,7 +5902,7 @@
         <v>567</v>
       </c>
       <c r="J27" s="250"/>
-      <c r="K27" s="345"/>
+      <c r="K27" s="356"/>
       <c r="L27" s="278"/>
       <c r="M27" s="157"/>
       <c r="N27" s="16"/>
@@ -5868,7 +5937,7 @@
         <v>563</v>
       </c>
       <c r="J28" s="250"/>
-      <c r="K28" s="345"/>
+      <c r="K28" s="312"/>
       <c r="L28" s="278"/>
       <c r="M28" s="157"/>
       <c r="N28" s="16"/>
@@ -5908,8 +5977,10 @@
       <c r="I29" s="39" t="s">
         <v>578</v>
       </c>
-      <c r="J29" s="298"/>
-      <c r="K29" s="344"/>
+      <c r="J29" s="298" t="s">
+        <v>615</v>
+      </c>
+      <c r="K29" s="311"/>
       <c r="L29" s="274" t="s">
         <v>409</v>
       </c>
@@ -5969,8 +6040,10 @@
       <c r="I30" s="39" t="s">
         <v>570</v>
       </c>
-      <c r="J30" s="298"/>
-      <c r="K30" s="344"/>
+      <c r="J30" s="298" t="s">
+        <v>614</v>
+      </c>
+      <c r="K30" s="311"/>
       <c r="L30" s="279" t="s">
         <v>427</v>
       </c>
@@ -6017,15 +6090,21 @@
       <c r="F31" s="263" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="293"/>
+      <c r="G31" s="357" t="s">
+        <v>112</v>
+      </c>
       <c r="H31" s="297" t="s">
         <v>18</v>
       </c>
       <c r="I31" s="39" t="s">
         <v>538</v>
       </c>
-      <c r="J31" s="294"/>
-      <c r="K31" s="341"/>
+      <c r="J31" s="298" t="s">
+        <v>617</v>
+      </c>
+      <c r="K31" s="311" t="s">
+        <v>616</v>
+      </c>
       <c r="L31" s="279" t="s">
         <v>427</v>
       </c>
@@ -6070,7 +6149,7 @@
       <c r="H32" s="287"/>
       <c r="I32" s="287"/>
       <c r="J32" s="294"/>
-      <c r="K32" s="341"/>
+      <c r="K32" s="308"/>
       <c r="L32" s="274" t="s">
         <v>409</v>
       </c>
@@ -6125,7 +6204,7 @@
         <v>567</v>
       </c>
       <c r="J33" s="250"/>
-      <c r="K33" s="345"/>
+      <c r="K33" s="312"/>
       <c r="L33" s="278"/>
       <c r="M33" s="157"/>
       <c r="N33" s="16"/>
@@ -6160,7 +6239,7 @@
         <v>563</v>
       </c>
       <c r="J34" s="250"/>
-      <c r="K34" s="345"/>
+      <c r="K34" s="312"/>
       <c r="L34" s="278"/>
       <c r="M34" s="157"/>
       <c r="N34" s="16"/>
@@ -6195,7 +6274,7 @@
       <c r="H35" s="287"/>
       <c r="I35" s="287"/>
       <c r="J35" s="294"/>
-      <c r="K35" s="341"/>
+      <c r="K35" s="308"/>
       <c r="L35" s="274" t="s">
         <v>409</v>
       </c>
@@ -6250,7 +6329,7 @@
       <c r="H36" s="287"/>
       <c r="I36" s="287"/>
       <c r="J36" s="294"/>
-      <c r="K36" s="341"/>
+      <c r="K36" s="308"/>
       <c r="L36" s="274" t="s">
         <v>409</v>
       </c>
@@ -6302,16 +6381,20 @@
         <v>117</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="H37" s="181" t="s">
         <v>446</v>
       </c>
       <c r="I37" s="256" t="s">
-        <v>602</v>
-      </c>
-      <c r="J37" s="257"/>
-      <c r="K37" s="343"/>
+        <v>600</v>
+      </c>
+      <c r="J37" s="310" t="s">
+        <v>618</v>
+      </c>
+      <c r="K37" s="257" t="s">
+        <v>619</v>
+      </c>
       <c r="L37" s="274" t="s">
         <v>409</v>
       </c>
@@ -6371,7 +6454,7 @@
       <c r="H38" s="287"/>
       <c r="I38" s="287"/>
       <c r="J38" s="294"/>
-      <c r="K38" s="341"/>
+      <c r="K38" s="308"/>
       <c r="L38" s="280" t="s">
         <v>432</v>
       </c>
@@ -6420,7 +6503,7 @@
       <c r="H39" s="287"/>
       <c r="I39" s="287"/>
       <c r="J39" s="294"/>
-      <c r="K39" s="341"/>
+      <c r="K39" s="308"/>
       <c r="L39" s="280" t="s">
         <v>435</v>
       </c>
@@ -6475,7 +6558,7 @@
       <c r="H40" s="287"/>
       <c r="I40" s="287"/>
       <c r="J40" s="294"/>
-      <c r="K40" s="341"/>
+      <c r="K40" s="308"/>
       <c r="L40" s="276" t="s">
         <v>437</v>
       </c>
@@ -6540,7 +6623,7 @@
       <c r="J41" s="300" t="s">
         <v>584</v>
       </c>
-      <c r="K41" s="346"/>
+      <c r="K41" s="313"/>
       <c r="L41" s="277" t="s">
         <v>420</v>
       </c>
@@ -6605,7 +6688,7 @@
       <c r="J42" s="300" t="s">
         <v>585</v>
       </c>
-      <c r="K42" s="346"/>
+      <c r="K42" s="313"/>
       <c r="L42" s="275" t="s">
         <v>427</v>
       </c>
@@ -6670,7 +6753,7 @@
       <c r="J43" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K43" s="347"/>
+      <c r="K43" s="314"/>
       <c r="L43" s="274" t="s">
         <v>409</v>
       </c>
@@ -6731,7 +6814,7 @@
         <v>581</v>
       </c>
       <c r="J44" s="41"/>
-      <c r="K44" s="348"/>
+      <c r="K44" s="315"/>
       <c r="L44" s="274" t="s">
         <v>409</v>
       </c>
@@ -6792,7 +6875,7 @@
         <v>582</v>
       </c>
       <c r="J45" s="41"/>
-      <c r="K45" s="348"/>
+      <c r="K45" s="315"/>
       <c r="L45" s="274" t="s">
         <v>409</v>
       </c>
@@ -6847,7 +6930,7 @@
         <v>567</v>
       </c>
       <c r="J46" s="250"/>
-      <c r="K46" s="345"/>
+      <c r="K46" s="312"/>
       <c r="L46" s="278"/>
       <c r="M46" s="157"/>
       <c r="N46" s="16"/>
@@ -6882,7 +6965,7 @@
         <v>563</v>
       </c>
       <c r="J47" s="250"/>
-      <c r="K47" s="345"/>
+      <c r="K47" s="312"/>
       <c r="L47" s="278"/>
       <c r="M47" s="157"/>
       <c r="N47" s="16"/>
@@ -6925,7 +7008,9 @@
       <c r="J48" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K48" s="347"/>
+      <c r="K48" s="314" t="s">
+        <v>620</v>
+      </c>
       <c r="L48" s="277" t="s">
         <v>420</v>
       </c>
@@ -6992,7 +7077,9 @@
       <c r="J49" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K49" s="347"/>
+      <c r="K49" s="314" t="s">
+        <v>621</v>
+      </c>
       <c r="L49" s="277" t="s">
         <v>420</v>
       </c>
@@ -7055,7 +7142,7 @@
         <v>594</v>
       </c>
       <c r="J50" s="301"/>
-      <c r="K50" s="347"/>
+      <c r="K50" s="314"/>
       <c r="L50" s="277" t="s">
         <v>420</v>
       </c>
@@ -7100,7 +7187,7 @@
       <c r="H51" s="288"/>
       <c r="I51" s="288"/>
       <c r="J51" s="291"/>
-      <c r="K51" s="349"/>
+      <c r="K51" s="316"/>
       <c r="L51" s="277" t="s">
         <v>420</v>
       </c>
@@ -7142,16 +7229,18 @@
         <v>101</v>
       </c>
       <c r="G52" s="295" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H52" s="181" t="s">
         <v>446</v>
       </c>
       <c r="I52" s="49" t="s">
-        <v>604</v>
-      </c>
-      <c r="J52" s="45"/>
-      <c r="K52" s="350"/>
+        <v>602</v>
+      </c>
+      <c r="J52" s="45" t="s">
+        <v>622</v>
+      </c>
+      <c r="K52" s="317"/>
       <c r="L52" s="277" t="s">
         <v>420</v>
       </c>
@@ -7199,10 +7288,12 @@
         <v>446</v>
       </c>
       <c r="I53" s="237" t="s">
-        <v>605</v>
-      </c>
-      <c r="J53" s="301"/>
-      <c r="K53" s="347"/>
+        <v>603</v>
+      </c>
+      <c r="J53" s="301" t="s">
+        <v>625</v>
+      </c>
+      <c r="K53" s="314"/>
       <c r="L53" s="276" t="s">
         <v>457</v>
       </c>
@@ -7254,10 +7345,12 @@
         <v>446</v>
       </c>
       <c r="I54" s="237" t="s">
-        <v>606</v>
-      </c>
-      <c r="J54" s="301"/>
-      <c r="K54" s="347"/>
+        <v>604</v>
+      </c>
+      <c r="J54" s="301" t="s">
+        <v>624</v>
+      </c>
+      <c r="K54" s="314"/>
       <c r="L54" s="274" t="s">
         <v>409</v>
       </c>
@@ -7302,7 +7395,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="7"/>
-      <c r="K55" s="351"/>
+      <c r="K55" s="318"/>
       <c r="L55" s="274" t="s">
         <v>409</v>
       </c>
@@ -7349,7 +7442,7 @@
         <v>571</v>
       </c>
       <c r="J56" s="305"/>
-      <c r="K56" s="352"/>
+      <c r="K56" s="319"/>
       <c r="L56" s="281" t="s">
         <v>460</v>
       </c>
@@ -7411,8 +7504,10 @@
       <c r="I57" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="J57" s="41"/>
-      <c r="K57" s="348"/>
+      <c r="J57" s="41" t="s">
+        <v>623</v>
+      </c>
+      <c r="K57" s="315"/>
       <c r="L57" s="282" t="s">
         <v>464</v>
       </c>
@@ -7474,8 +7569,10 @@
       <c r="I58" s="44" t="s">
         <v>573</v>
       </c>
-      <c r="J58" s="41"/>
-      <c r="K58" s="348"/>
+      <c r="J58" s="41" t="s">
+        <v>623</v>
+      </c>
+      <c r="K58" s="315"/>
       <c r="L58" s="282" t="s">
         <v>468</v>
       </c>
@@ -7534,7 +7631,7 @@
         <v>574</v>
       </c>
       <c r="J59" s="97"/>
-      <c r="K59" s="342"/>
+      <c r="K59" s="309"/>
       <c r="L59" s="281" t="s">
         <v>469</v>
       </c>
@@ -7591,7 +7688,7 @@
       <c r="H60" s="287"/>
       <c r="I60" s="287"/>
       <c r="J60" s="294"/>
-      <c r="K60" s="341"/>
+      <c r="K60" s="308"/>
       <c r="L60" s="277" t="s">
         <v>420</v>
       </c>
@@ -7648,7 +7745,7 @@
         <v>575</v>
       </c>
       <c r="J61" s="45"/>
-      <c r="K61" s="350"/>
+      <c r="K61" s="317"/>
       <c r="L61" s="283" t="s">
         <v>473</v>
       </c>
@@ -7703,7 +7800,7 @@
         <v>567</v>
       </c>
       <c r="J62" s="250"/>
-      <c r="K62" s="345"/>
+      <c r="K62" s="312"/>
       <c r="L62" s="278"/>
       <c r="M62" s="157"/>
       <c r="N62" s="16"/>
@@ -7738,7 +7835,7 @@
         <v>563</v>
       </c>
       <c r="J63" s="250"/>
-      <c r="K63" s="345"/>
+      <c r="K63" s="312"/>
       <c r="L63" s="278"/>
       <c r="M63" s="157"/>
       <c r="N63" s="16"/>
@@ -7775,7 +7872,7 @@
         <v>576</v>
       </c>
       <c r="J64" s="45"/>
-      <c r="K64" s="350"/>
+      <c r="K64" s="317"/>
       <c r="L64" s="283" t="s">
         <v>475</v>
       </c>
@@ -7830,7 +7927,7 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
       <c r="J65" s="7"/>
-      <c r="K65" s="351"/>
+      <c r="K65" s="318"/>
       <c r="L65" s="275" t="s">
         <v>427</v>
       </c>
@@ -7889,7 +7986,7 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="J66" s="7"/>
-      <c r="K66" s="351"/>
+      <c r="K66" s="318"/>
       <c r="L66" s="274" t="s">
         <v>409</v>
       </c>
@@ -7944,7 +8041,7 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
       <c r="J67" s="7"/>
-      <c r="K67" s="351"/>
+      <c r="K67" s="318"/>
       <c r="L67" s="274" t="s">
         <v>409</v>
       </c>
@@ -7999,7 +8096,7 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="J68" s="7"/>
-      <c r="K68" s="351"/>
+      <c r="K68" s="318"/>
       <c r="L68" s="274" t="s">
         <v>409</v>
       </c>
@@ -8054,7 +8151,7 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
       <c r="J69" s="7"/>
-      <c r="K69" s="351"/>
+      <c r="K69" s="318"/>
       <c r="L69" s="274" t="s">
         <v>409</v>
       </c>
@@ -8117,7 +8214,7 @@
       <c r="J70" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K70" s="347"/>
+      <c r="K70" s="314"/>
       <c r="L70" s="274" t="s">
         <v>409</v>
       </c>
@@ -8180,7 +8277,7 @@
       <c r="J71" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K71" s="347"/>
+      <c r="K71" s="314"/>
       <c r="L71" s="284" t="s">
         <v>480</v>
       </c>
@@ -8237,7 +8334,7 @@
       <c r="H72" s="287"/>
       <c r="I72" s="287"/>
       <c r="J72" s="294"/>
-      <c r="K72" s="341"/>
+      <c r="K72" s="308"/>
       <c r="L72" s="274" t="s">
         <v>409</v>
       </c>
@@ -8295,12 +8392,12 @@
         <v>446</v>
       </c>
       <c r="I73" s="237" t="s">
+        <v>559</v>
+      </c>
+      <c r="J73" s="301" t="s">
         <v>598</v>
       </c>
-      <c r="J73" s="301" t="s">
-        <v>600</v>
-      </c>
-      <c r="K73" s="347"/>
+      <c r="K73" s="314"/>
       <c r="L73" s="284" t="s">
         <v>485</v>
       </c>
@@ -8358,12 +8455,12 @@
         <v>588</v>
       </c>
       <c r="I74" s="237" t="s">
-        <v>599</v>
+        <v>558</v>
       </c>
       <c r="J74" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K74" s="347"/>
+      <c r="K74" s="314"/>
       <c r="L74" s="274" t="s">
         <v>409</v>
       </c>
@@ -8416,7 +8513,7 @@
         <v>567</v>
       </c>
       <c r="J75" s="250"/>
-      <c r="K75" s="345"/>
+      <c r="K75" s="312"/>
       <c r="L75" s="278" t="s">
         <v>487</v>
       </c>
@@ -8459,7 +8556,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
       <c r="J76" s="7"/>
-      <c r="K76" s="351"/>
+      <c r="K76" s="318"/>
       <c r="L76" s="277" t="s">
         <v>420</v>
       </c>
@@ -8528,7 +8625,7 @@
       <c r="J77" s="301" t="s">
         <v>587</v>
       </c>
-      <c r="K77" s="347"/>
+      <c r="K77" s="314"/>
       <c r="L77" s="284" t="s">
         <v>492</v>
       </c>
@@ -8587,7 +8684,7 @@
         <v>567</v>
       </c>
       <c r="J78" s="250"/>
-      <c r="K78" s="345"/>
+      <c r="K78" s="312"/>
       <c r="L78" s="278"/>
       <c r="M78" s="157"/>
       <c r="N78" s="16"/>
@@ -8622,7 +8719,7 @@
         <v>563</v>
       </c>
       <c r="J79" s="252"/>
-      <c r="K79" s="353"/>
+      <c r="K79" s="320"/>
       <c r="L79" s="285"/>
       <c r="M79" s="195"/>
       <c r="N79" s="17"/>
@@ -8840,6 +8937,16 @@
   </sheetData>
   <autoFilter ref="B15:X79" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="26">
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="N14:R14"/>
     <mergeCell ref="U14:X14"/>
@@ -8856,16 +8963,6 @@
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E22:F22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10951,31 +11048,31 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B3" s="335" t="s">
+      <c r="B3" s="351" t="s">
         <v>317</v>
       </c>
-      <c r="C3" s="337" t="s">
+      <c r="C3" s="353" t="s">
         <v>514</v>
       </c>
-      <c r="D3" s="338"/>
-      <c r="E3" s="333" t="s">
+      <c r="D3" s="354"/>
+      <c r="E3" s="349" t="s">
         <v>515</v>
       </c>
-      <c r="F3" s="334"/>
-      <c r="H3" s="335" t="s">
+      <c r="F3" s="350"/>
+      <c r="H3" s="351" t="s">
         <v>317</v>
       </c>
-      <c r="I3" s="337" t="s">
+      <c r="I3" s="353" t="s">
         <v>514</v>
       </c>
-      <c r="J3" s="338"/>
-      <c r="K3" s="333" t="s">
+      <c r="J3" s="354"/>
+      <c r="K3" s="349" t="s">
         <v>515</v>
       </c>
-      <c r="L3" s="334"/>
+      <c r="L3" s="350"/>
     </row>
     <row r="4" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="336"/>
+      <c r="B4" s="352"/>
       <c r="C4" s="209" t="s">
         <v>513</v>
       </c>
@@ -10988,7 +11085,7 @@
       <c r="F4" s="216" t="s">
         <v>516</v>
       </c>
-      <c r="H4" s="336"/>
+      <c r="H4" s="352"/>
       <c r="I4" s="209" t="s">
         <v>301</v>
       </c>

</xml_diff>